<commit_message>
wingo commander e world in conflict
</commit_message>
<xml_diff>
--- a/jogos.xlsx
+++ b/jogos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\mycollections-cli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29C46EB-922B-40C6-9AF0-FD4853AB55FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F047B37-2103-4368-9F2C-1D3365400348}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{0C35237A-6EB4-4B02-9651-931FED775CEC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3522" uniqueCount="1395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3524" uniqueCount="1397">
   <si>
     <t>Dragon Age Origins</t>
   </si>
@@ -4216,6 +4216,12 @@
   </si>
   <si>
     <t>https://www.oficinadanet.com.br/imagens/post/18102/for-honor.jpg</t>
+  </si>
+  <si>
+    <t>http://www.mweb.co.za/DesktopModules/DigArticle/MediaHandler.ashx?portalid=20&amp;moduleid=5259&amp;mediaid=52965&amp;width=665&amp;height=400</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ6FucwiR-HCKJMJigIUR6g4vNSbsSXUtUPFgsxGOtNNeVL9eRZLA</t>
   </si>
 </sst>
 </file>
@@ -4589,8 +4595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E073D1A-5126-4785-A652-5C66939BBDE3}">
   <dimension ref="A1:F707"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="B218" sqref="B218"/>
+    <sheetView tabSelected="1" topLeftCell="A667" workbookViewId="0">
+      <selection activeCell="B691" sqref="B691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18020,6 +18026,9 @@
       <c r="A690" t="s">
         <v>139</v>
       </c>
+      <c r="B690" s="1" t="s">
+        <v>1396</v>
+      </c>
       <c r="C690" t="s">
         <v>1</v>
       </c>
@@ -18073,6 +18082,9 @@
     <row r="693" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
         <v>59</v>
+      </c>
+      <c r="B693" s="1" t="s">
+        <v>1395</v>
       </c>
       <c r="C693" t="s">
         <v>58</v>
@@ -18371,8 +18383,10 @@
     <hyperlink ref="B106" r:id="rId6" xr:uid="{419B2CD6-76F3-456C-894C-496997E3F2C1}"/>
     <hyperlink ref="B163" r:id="rId7" xr:uid="{F723D508-E6CE-40BC-960E-F2B1B9CA372B}"/>
     <hyperlink ref="B217" r:id="rId8" xr:uid="{FB40AEB8-DF48-4191-A4BC-673A6FD43EA3}"/>
+    <hyperlink ref="B693" r:id="rId9" xr:uid="{E69B2788-3231-4301-AA5A-C0EC9C810CA9}"/>
+    <hyperlink ref="B690" r:id="rId10" xr:uid="{AA568B96-FA0C-458D-8733-B95E26833E38}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
beyond good and evil
</commit_message>
<xml_diff>
--- a/jogos.xlsx
+++ b/jogos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\mycollections-cli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F047B37-2103-4368-9F2C-1D3365400348}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A290E5E2-47C8-4177-BD58-F446E3C2F6F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{0C35237A-6EB4-4B02-9651-931FED775CEC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3524" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3525" uniqueCount="1398">
   <si>
     <t>Dragon Age Origins</t>
   </si>
@@ -4222,6 +4222,9 @@
   </si>
   <si>
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ6FucwiR-HCKJMJigIUR6g4vNSbsSXUtUPFgsxGOtNNeVL9eRZLA</t>
+  </si>
+  <si>
+    <t>https://steamcdn-a.akamaihd.net/steam/apps/15130/header.jpg?t=1447351297</t>
   </si>
 </sst>
 </file>
@@ -4595,8 +4598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E073D1A-5126-4785-A652-5C66939BBDE3}">
   <dimension ref="A1:F707"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A667" workbookViewId="0">
-      <selection activeCell="B691" sqref="B691"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5589,6 +5592,9 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>84</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>1397</v>
       </c>
       <c r="C52" t="s">
         <v>58</v>
@@ -18385,8 +18391,9 @@
     <hyperlink ref="B217" r:id="rId8" xr:uid="{FB40AEB8-DF48-4191-A4BC-673A6FD43EA3}"/>
     <hyperlink ref="B693" r:id="rId9" xr:uid="{E69B2788-3231-4301-AA5A-C0EC9C810CA9}"/>
     <hyperlink ref="B690" r:id="rId10" xr:uid="{AA568B96-FA0C-458D-8733-B95E26833E38}"/>
+    <hyperlink ref="B52" r:id="rId11" xr:uid="{42256FEE-B4A9-42EE-A425-53B52A85F2F0}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
jogos ps3 e fix no downloadImages
</commit_message>
<xml_diff>
--- a/jogos.xlsx
+++ b/jogos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\mycollections-cli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF3B044-D62A-478D-9743-B32427D024B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92940F6-5864-42E2-B138-FBDA39D2BB45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{0C35237A-6EB4-4B02-9651-931FED775CEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3606" uniqueCount="1418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3702" uniqueCount="1462">
   <si>
     <t>Dragon Age Origins</t>
   </si>
@@ -4279,6 +4279,138 @@
   </si>
   <si>
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTUnXcMAHizEe3zP8NaFLtXgQqf1IvUkNdNL0Yfz0psWp4qP2rK9w</t>
+  </si>
+  <si>
+    <t>Ratchet and Clank All 4 One</t>
+  </si>
+  <si>
+    <t>Heavy Rain Movie Edition</t>
+  </si>
+  <si>
+    <t>Gran Turismo 5 XL Edition</t>
+  </si>
+  <si>
+    <t>Little Big Planet 2</t>
+  </si>
+  <si>
+    <t>Motorstorm</t>
+  </si>
+  <si>
+    <t>PES 2013</t>
+  </si>
+  <si>
+    <t>inFamous</t>
+  </si>
+  <si>
+    <t>Mortal Kombat</t>
+  </si>
+  <si>
+    <t>Killzone Trilogy</t>
+  </si>
+  <si>
+    <t>Gran Turismo 6</t>
+  </si>
+  <si>
+    <t>Red Dead Redemption</t>
+  </si>
+  <si>
+    <t>Beyond Two Souls</t>
+  </si>
+  <si>
+    <t>Dragon Age 2</t>
+  </si>
+  <si>
+    <t>Lost Planet Extreme Condition</t>
+  </si>
+  <si>
+    <t>God of War Collection</t>
+  </si>
+  <si>
+    <t>Midnight Club Log Angeles Complete Edition</t>
+  </si>
+  <si>
+    <t>Uncharted Drakes Fortune</t>
+  </si>
+  <si>
+    <t>The ICO Shadow of Colossus Collection</t>
+  </si>
+  <si>
+    <t>God of War Ascension</t>
+  </si>
+  <si>
+    <t>God of War 3</t>
+  </si>
+  <si>
+    <t>Uncharted 3 Drakes Deception</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTRm5XEFnZ71oYQLvAMQJ6A4tgfW2_gE6RsAca-aoSKl-acXmIW</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTe0_v-hOzSjRoRvLRZ4Ll20Nj1FKGQSfjwWya2olg1WDSMgFm9</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSwvdVJPIgLTc2giqWyKcinp0ulFm-A81beGE2akmU7SSBUY5G9</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSpk_RTsoY4jVMnQBqwTzzjW00Ls2Lb5KzZNOhsUlzlh57cJKXxQg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSDbrdfTrndAE9but-T0iF2GnCEO6lK8RQ1re1fCm4ChkPM2gooZA</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRZT6_X-qlUEGMuxU0lk776z52Mtxy2mmZ3taAJjGcOaa04-PeH</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTyZCJ5o2cMBRMobU-qldhJyYXUWqJGT4FJU1pJphzgDXms2ThSVA</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ7AAjB3c-VuhZvATzHNBRHs6r00wRt1SOvK5zJ5vixoBHEHLsL</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRa2cyjejKWx57Vfu2OpZHjB1Jbkn8CC8uCbwfMp3fhD6PljR5o-Q</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTzsUHfpvqJ1Dn6ZiPuShRJXTTHog7qf4Z_ttSUH6Bdv37GzqN3</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSLyExBvi23HGeKr5R5UgauBoP_DgP8_PVhmmWEt-6nul5K13FSBg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTR9AmwnSDcKC7w2CXPHnRVTSoaEm6QQMVNoakZDRAzYfYKtMGmlg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ_jakGPOZGqEuSdN6FRpKrhZCnQMZ4lYLe2fKorMYjpkyz0LNQ</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSQWOy0WXJL2e0bfDPZgdqO4Km355R2xmxWNNNSLg3vffF9YOLb</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTd79SqojbqNrRmf6a8cszFR7zoJRq26DlQ0DXtvA_oatKJR6fz</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcT20gHGrOmDYZx3xZ_EBb8EpRCJBeZzHgAKTCI7DTT4w94Yivue0g</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRcfiuqf8Cp3vq3nAeJhjDPU0sUQEced9FT4T_X3Agaqqdkjpxu</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTc9-osM_8ThlNZ6-7f_EYhk-qVnYZtoaPjLkTeXX56vo3VBUq_</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRMe8HaTwp-2-ENp3h6IatV3rZAG1oXIWIvz-aRp3sBLoeuBdul5A</t>
+  </si>
+  <si>
+    <t>Uncharted 2 Among thieves</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSrBzivi2eISmBFdA3CMHXlVeBThZickS_hINQl6WBfBvLCtv5UNA</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRS9TRkOnpVGNEt6CtJaOTEBxSEJbVo3ltV6AM2gNAS2Fge_c8FYw</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRwQfe_qAwJZyfhwwuXDjwFfKYx5kk4ovykayUOnEHQ0g1IFQNn</t>
   </si>
 </sst>
 </file>
@@ -4641,10 +4773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E073D1A-5126-4785-A652-5C66939BBDE3}">
-  <dimension ref="A1:F723"/>
+  <dimension ref="A1:F747"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A692" workbookViewId="0">
-      <selection activeCell="A685" sqref="A685"/>
+    <sheetView tabSelected="1" topLeftCell="A714" workbookViewId="0">
+      <selection activeCell="B744" sqref="B744"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18696,9 +18828,345 @@
         <v>230</v>
       </c>
     </row>
+    <row r="724" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A724" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B724" t="s">
+        <v>1439</v>
+      </c>
+      <c r="E724" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F724" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="725" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A725" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B725" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E725" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F725" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="726" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A726" t="s">
+        <v>85</v>
+      </c>
+      <c r="B726" t="s">
+        <v>86</v>
+      </c>
+      <c r="E726" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F726" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="727" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A727" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B727" t="s">
+        <v>1441</v>
+      </c>
+      <c r="E727" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F727" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="728" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A728" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B728" t="s">
+        <v>1442</v>
+      </c>
+      <c r="E728" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F728" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="729" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A729" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B729" t="s">
+        <v>1443</v>
+      </c>
+      <c r="E729" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F729" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="730" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A730" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B730" t="s">
+        <v>1444</v>
+      </c>
+      <c r="E730" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F730" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="731" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A731" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B731" t="s">
+        <v>1445</v>
+      </c>
+      <c r="E731" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F731" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="732" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A732" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B732" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E732" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F732" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="733" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A733" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B733" t="s">
+        <v>1447</v>
+      </c>
+      <c r="E733" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F733" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="734" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A734" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B734" t="s">
+        <v>1448</v>
+      </c>
+      <c r="E734" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F734" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="735" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A735" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B735" t="s">
+        <v>1449</v>
+      </c>
+      <c r="E735" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F735" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="736" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A736" t="s">
+        <v>806</v>
+      </c>
+      <c r="B736" t="s">
+        <v>1450</v>
+      </c>
+      <c r="E736" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F736" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="737" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A737" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B737" t="s">
+        <v>1451</v>
+      </c>
+      <c r="E737" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F737" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="738" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A738" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B738" t="s">
+        <v>1452</v>
+      </c>
+      <c r="E738" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F738" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="739" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A739" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B739" t="s">
+        <v>755</v>
+      </c>
+      <c r="E739" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F739" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="740" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A740" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B740" t="s">
+        <v>1453</v>
+      </c>
+      <c r="E740" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F740" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="741" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A741" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B741" t="s">
+        <v>1454</v>
+      </c>
+      <c r="E741" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F741" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="742" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A742" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B742" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E742" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F742" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="743" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A743" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B743" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E743" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F743" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="744" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A744" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B744" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E744" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F744" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="745" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A745" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B745" t="s">
+        <v>1459</v>
+      </c>
+      <c r="E745" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F745" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="746" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A746" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B746" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E746" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F746" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="747" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A747" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B747" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E747" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F747" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F707">
-    <sortCondition ref="A2"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A724:A747">
+    <sortCondition ref="A724"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1" xr:uid="{2726AE12-75BD-43F3-877F-718C53B6A31E}"/>

</xml_diff>

<commit_message>
PS4 e Xbox One
</commit_message>
<xml_diff>
--- a/jogos.xlsx
+++ b/jogos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\mycollections-cli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92940F6-5864-42E2-B138-FBDA39D2BB45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4CB371-DA3F-448C-BCA7-08112F72BDA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{0C35237A-6EB4-4B02-9651-931FED775CEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3702" uniqueCount="1462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3911" uniqueCount="1527">
   <si>
     <t>Dragon Age Origins</t>
   </si>
@@ -4411,6 +4411,201 @@
   </si>
   <si>
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRwQfe_qAwJZyfhwwuXDjwFfKYx5kk4ovykayUOnEHQ0g1IFQNn</t>
+  </si>
+  <si>
+    <t>Mídia Física</t>
+  </si>
+  <si>
+    <t>PES 2018</t>
+  </si>
+  <si>
+    <t>The Order 1886</t>
+  </si>
+  <si>
+    <t>Killzone Shadow Fall</t>
+  </si>
+  <si>
+    <t>Infamous Second Son</t>
+  </si>
+  <si>
+    <t>DriveClub</t>
+  </si>
+  <si>
+    <t>Far Cry 4</t>
+  </si>
+  <si>
+    <t>Call of Duty Advanced Warfare</t>
+  </si>
+  <si>
+    <t>FIFA 14</t>
+  </si>
+  <si>
+    <t>NBA 2K14</t>
+  </si>
+  <si>
+    <t>The Last of Us Remastered</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto 5</t>
+  </si>
+  <si>
+    <t>Assassins Creed Syndicate</t>
+  </si>
+  <si>
+    <t>Ratchet and Clank</t>
+  </si>
+  <si>
+    <t>Evolve</t>
+  </si>
+  <si>
+    <t>Bloodborne</t>
+  </si>
+  <si>
+    <t>Horizon Zero Dawn</t>
+  </si>
+  <si>
+    <t>Dark Souls 3</t>
+  </si>
+  <si>
+    <t>Gran Turismo Sport</t>
+  </si>
+  <si>
+    <t>Red Dead Redemption 2</t>
+  </si>
+  <si>
+    <t>PS4</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcThDPDmdYWLV30hYNX-h3M7VJZNOWhJUf-sZ2JUAX6E4DaiJa2b</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ8YBCVG9Vek1UTKiHbhNJzUEG8WOk38hPy-NoiOVWqeBf66Uuwfw</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTFlC-2e0cG4bzb-XCP-1DvpGoL_TnfoodEKE3TuOf69ubWUAbrsw</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSL9z3MbvM5z7A6CI79kLfxrIh4Yr4breMyuZT0yo-lhUitHeL-jA</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSEvgOwLofhyFRx1ToodvRnsZT_msvtzQI1t1aMO-kTIaP4cl-4</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTx0-4nKjoqh2szgJa30HAq5LidZEY4s4WwYGDwi0H94W918giBog</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSRlRmqt2RV45uLRj6lhYakRTsglF_B96uj72yV9ujStdjqKsiE</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcR-OKyM1DUuk06uI7U5abLssZ7AYCSJrGybauDUbK3arb1KIuZp</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSL_M7lh8PH9S1OyFMfwyhl4FAAUIGY1LcmeVfxQT3ux3tTGi-46Q</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSUvv7eYbgjnlVTW7cS58wsYbxbewIxfRei1a0fHQcw4wsy14QnAA</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRuqVu6_9I_ZgH1f7DpObYqQ2LepVcHufU5K46p6A_EJfjWeqR0</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcT_gIUCWGtlAGBBqRAvW2k3Z0Nkp1RS7rOKjSisL5fLZGKB8Wma7w</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRRkA2Lzh2Nr8f1IxcaWr9fzVG8ZJBdgL9nASxZX3OhEN4_Qe1V</t>
+  </si>
+  <si>
+    <t>Uncharted 4 A Thiefs End</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTCgb2dAW09y_DdFt6ryRL9f1zBmnJdhk4a3cLQcw0eJQonEDQt</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRAggmdCtsIRgA--TjWbzS27ad3vkk88sfWU25-VteDoCoOHl9bHQ</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSnk5Q2XLKSSFwoJQ_QTMIER3UqdOiCZuZYFuzVamvQaGoEo8vj</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTLcYjo6_ZVZgiYqeQDhEXDzc3BCD9CQcUnWcJKwU-ptUBcYpmQgA</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQPJHPkiz8giw0FrzO8RxjPuC0nvUDVm1Y_8nuDpH6VPatekCkQWA</t>
+  </si>
+  <si>
+    <t>https://4gnews.pt/wp-content/uploads/2018/10/red-dead-redemption-ii-3755-600.jpg</t>
+  </si>
+  <si>
+    <t>Metal Gear Solid The Phantom Pain</t>
+  </si>
+  <si>
+    <t>PES 2016</t>
+  </si>
+  <si>
+    <t>Halo 5</t>
+  </si>
+  <si>
+    <t>Dead Rising 3</t>
+  </si>
+  <si>
+    <t>Sunset Overdrive</t>
+  </si>
+  <si>
+    <t>Gear of War Ultimate Edition</t>
+  </si>
+  <si>
+    <t>Rise of Tomb Raider</t>
+  </si>
+  <si>
+    <t>Dragon Age Inquisition</t>
+  </si>
+  <si>
+    <t>Titanfall</t>
+  </si>
+  <si>
+    <t>Forza 5</t>
+  </si>
+  <si>
+    <t>Dead Rising 4</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ-Lmi5qcc73NBQE0JKaoF5215snYJ11oHeGZiEyfXZjZQhNPtzsg</t>
+  </si>
+  <si>
+    <t>Crash Bandicoot Insane Trilogy</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRjGK3V4s8dLLdMaDZBSMsnPp94oH9-v7FsAobLJ97PTnOyd_Jl</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcT53Le6Q7zXkK5YoZjLVv1JFYzN95zdkmCe8VQYHJM7FlxONl0h5g</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcT-fl98YBgZACbeM18QXYNRWo0NxtbuwhY-dk9BZF_6cQkg68Q4</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQdg2-XlMqwUeIKmx4Iil-CMAind2I_vHr4heHuIuzKChAxSRNf</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcS-RdlN-WZrzy3J65F9jcQbf1eA9Z8zmVX09au3gu1RbbaN90Nk</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRMGtEusWY1gxQZxJ_M1qVsXdtczEkbr1hAH1R0Giaj6BcSxpS3</t>
+  </si>
+  <si>
+    <t>https://www.meups4.com.br/wp-content/uploads/2015/03/Metal-Gear-Solid-V-The-Phantom-Pain1.jpg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ2iMubiGIAgXAbiLfP0YOJ78mD2sKz5IYBUb_naRyvLH-U8db54Q</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcR_0VLGXdPQyXlXOEOkThmsEkU3FgJfnbzP3CZtvIwCS1KUU5raDg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTixF7cMbyljJbluC5z9wWQ65tZNWAKCdCfjfJCJuguq8_iHXUtUQ</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcR4KZPqO_tC9D-dLTCplwUlLBgM322UKKzRWHkIu1RWHK71D2UX</t>
   </si>
 </sst>
 </file>
@@ -4773,10 +4968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E073D1A-5126-4785-A652-5C66939BBDE3}">
-  <dimension ref="A1:F747"/>
+  <dimension ref="A1:F784"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A714" workbookViewId="0">
-      <selection activeCell="B744" sqref="B744"/>
+    <sheetView tabSelected="1" topLeftCell="A762" workbookViewId="0">
+      <selection activeCell="B784" sqref="B784"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18835,6 +19030,9 @@
       <c r="B724" t="s">
         <v>1439</v>
       </c>
+      <c r="C724" t="s">
+        <v>1462</v>
+      </c>
       <c r="E724" t="s">
         <v>1398</v>
       </c>
@@ -18849,6 +19047,9 @@
       <c r="B725" t="s">
         <v>1440</v>
       </c>
+      <c r="C725" t="s">
+        <v>1462</v>
+      </c>
       <c r="E725" t="s">
         <v>1398</v>
       </c>
@@ -18863,6 +19064,9 @@
       <c r="B726" t="s">
         <v>86</v>
       </c>
+      <c r="C726" t="s">
+        <v>1462</v>
+      </c>
       <c r="E726" t="s">
         <v>1398</v>
       </c>
@@ -18877,6 +19081,9 @@
       <c r="B727" t="s">
         <v>1441</v>
       </c>
+      <c r="C727" t="s">
+        <v>1462</v>
+      </c>
       <c r="E727" t="s">
         <v>1398</v>
       </c>
@@ -18891,6 +19098,9 @@
       <c r="B728" t="s">
         <v>1442</v>
       </c>
+      <c r="C728" t="s">
+        <v>1462</v>
+      </c>
       <c r="E728" t="s">
         <v>1398</v>
       </c>
@@ -18905,6 +19115,9 @@
       <c r="B729" t="s">
         <v>1443</v>
       </c>
+      <c r="C729" t="s">
+        <v>1462</v>
+      </c>
       <c r="E729" t="s">
         <v>1398</v>
       </c>
@@ -18919,6 +19132,9 @@
       <c r="B730" t="s">
         <v>1444</v>
       </c>
+      <c r="C730" t="s">
+        <v>1462</v>
+      </c>
       <c r="E730" t="s">
         <v>1398</v>
       </c>
@@ -18933,6 +19149,9 @@
       <c r="B731" t="s">
         <v>1445</v>
       </c>
+      <c r="C731" t="s">
+        <v>1462</v>
+      </c>
       <c r="E731" t="s">
         <v>1398</v>
       </c>
@@ -18947,6 +19166,9 @@
       <c r="B732" t="s">
         <v>1446</v>
       </c>
+      <c r="C732" t="s">
+        <v>1462</v>
+      </c>
       <c r="E732" t="s">
         <v>1398</v>
       </c>
@@ -18961,6 +19183,9 @@
       <c r="B733" t="s">
         <v>1447</v>
       </c>
+      <c r="C733" t="s">
+        <v>1462</v>
+      </c>
       <c r="E733" t="s">
         <v>1398</v>
       </c>
@@ -18975,6 +19200,9 @@
       <c r="B734" t="s">
         <v>1448</v>
       </c>
+      <c r="C734" t="s">
+        <v>1462</v>
+      </c>
       <c r="E734" t="s">
         <v>1398</v>
       </c>
@@ -18989,6 +19217,9 @@
       <c r="B735" t="s">
         <v>1449</v>
       </c>
+      <c r="C735" t="s">
+        <v>1462</v>
+      </c>
       <c r="E735" t="s">
         <v>1398</v>
       </c>
@@ -19003,6 +19234,9 @@
       <c r="B736" t="s">
         <v>1450</v>
       </c>
+      <c r="C736" t="s">
+        <v>1462</v>
+      </c>
       <c r="E736" t="s">
         <v>1398</v>
       </c>
@@ -19017,6 +19251,9 @@
       <c r="B737" t="s">
         <v>1451</v>
       </c>
+      <c r="C737" t="s">
+        <v>1462</v>
+      </c>
       <c r="E737" t="s">
         <v>1398</v>
       </c>
@@ -19031,6 +19268,9 @@
       <c r="B738" t="s">
         <v>1452</v>
       </c>
+      <c r="C738" t="s">
+        <v>1462</v>
+      </c>
       <c r="E738" t="s">
         <v>1398</v>
       </c>
@@ -19045,6 +19285,9 @@
       <c r="B739" t="s">
         <v>755</v>
       </c>
+      <c r="C739" t="s">
+        <v>1462</v>
+      </c>
       <c r="E739" t="s">
         <v>1398</v>
       </c>
@@ -19059,6 +19302,9 @@
       <c r="B740" t="s">
         <v>1453</v>
       </c>
+      <c r="C740" t="s">
+        <v>1462</v>
+      </c>
       <c r="E740" t="s">
         <v>1398</v>
       </c>
@@ -19073,6 +19319,9 @@
       <c r="B741" t="s">
         <v>1454</v>
       </c>
+      <c r="C741" t="s">
+        <v>1462</v>
+      </c>
       <c r="E741" t="s">
         <v>1398</v>
       </c>
@@ -19087,6 +19336,9 @@
       <c r="B742" t="s">
         <v>1455</v>
       </c>
+      <c r="C742" t="s">
+        <v>1462</v>
+      </c>
       <c r="E742" t="s">
         <v>1398</v>
       </c>
@@ -19101,6 +19353,9 @@
       <c r="B743" t="s">
         <v>1456</v>
       </c>
+      <c r="C743" t="s">
+        <v>1462</v>
+      </c>
       <c r="E743" t="s">
         <v>1398</v>
       </c>
@@ -19115,6 +19370,9 @@
       <c r="B744" t="s">
         <v>1457</v>
       </c>
+      <c r="C744" t="s">
+        <v>1462</v>
+      </c>
       <c r="E744" t="s">
         <v>1398</v>
       </c>
@@ -19129,6 +19387,9 @@
       <c r="B745" t="s">
         <v>1459</v>
       </c>
+      <c r="C745" t="s">
+        <v>1462</v>
+      </c>
       <c r="E745" t="s">
         <v>1398</v>
       </c>
@@ -19143,6 +19404,9 @@
       <c r="B746" t="s">
         <v>1460</v>
       </c>
+      <c r="C746" t="s">
+        <v>1462</v>
+      </c>
       <c r="E746" t="s">
         <v>1398</v>
       </c>
@@ -19157,6 +19421,9 @@
       <c r="B747" t="s">
         <v>1461</v>
       </c>
+      <c r="C747" t="s">
+        <v>1462</v>
+      </c>
       <c r="E747" t="s">
         <v>1398</v>
       </c>
@@ -19164,9 +19431,638 @@
         <v>230</v>
       </c>
     </row>
+    <row r="748" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A748" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B748" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C748" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E748" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F748" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="749" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A749" t="s">
+        <v>211</v>
+      </c>
+      <c r="B749" t="s">
+        <v>212</v>
+      </c>
+      <c r="C749" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E749" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F749" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="750" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A750" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B750" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C750" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E750" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F750" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="751" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A751" t="s">
+        <v>1469</v>
+      </c>
+      <c r="B751" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C751" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E751" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F751" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="752" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A752" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B752" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C752" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E752" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F752" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="753" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A753" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B753" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C753" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E753" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F753" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="754" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A754" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B754" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C754" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E754" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F754" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="755" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A755" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B755" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C755" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E755" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F755" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="756" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A756" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B756" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C756" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E756" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F756" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="757" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A757" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B757" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C757" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E757" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F757" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="758" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A758" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B758" t="s">
+        <v>193</v>
+      </c>
+      <c r="C758" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E758" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F758" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="759" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A759" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B759" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C759" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E759" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F759" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="760" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A760" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B760" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C760" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E760" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F760" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="761" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A761" t="s">
+        <v>1465</v>
+      </c>
+      <c r="B761" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C761" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E761" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F761" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="762" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A762" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B762" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C762" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E762" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F762" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="763" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A763" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B763" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C763" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E763" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F763" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="764" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A764" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B764" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C764" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E764" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F764" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="765" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A765" t="s">
+        <v>90</v>
+      </c>
+      <c r="B765" t="s">
+        <v>91</v>
+      </c>
+      <c r="C765" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E765" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F765" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="766" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A766" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B766" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C766" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E766" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F766" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="767" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A767" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B767" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C767" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E767" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F767" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="768" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A768" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B768" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C768" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E768" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F768" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="769" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A769" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B769" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C769" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E769" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F769" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="770" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A770" t="s">
+        <v>57</v>
+      </c>
+      <c r="B770" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C770" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E770" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F770" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="771" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A771" t="s">
+        <v>120</v>
+      </c>
+      <c r="B771" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C771" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E771" t="s">
+        <v>171</v>
+      </c>
+      <c r="F771" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="772" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A772" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B772" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C772" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E772" t="s">
+        <v>171</v>
+      </c>
+      <c r="F772" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="773" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A773" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B773" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C773" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E773" t="s">
+        <v>171</v>
+      </c>
+      <c r="F773" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="774" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A774" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B774" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C774" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E774" t="s">
+        <v>171</v>
+      </c>
+      <c r="F774" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="775" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A775" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B775" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C775" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E775" t="s">
+        <v>171</v>
+      </c>
+      <c r="F775" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="776" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A776" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B776" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C776" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E776" t="s">
+        <v>171</v>
+      </c>
+      <c r="F776" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="777" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A777" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B777" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C777" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E777" t="s">
+        <v>171</v>
+      </c>
+      <c r="F777" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="778" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A778" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B778" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C778" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E778" t="s">
+        <v>171</v>
+      </c>
+      <c r="F778" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="779" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A779" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B779" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C779" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E779" t="s">
+        <v>171</v>
+      </c>
+      <c r="F779" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="780" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A780" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B780" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C780" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E780" t="s">
+        <v>171</v>
+      </c>
+      <c r="F780" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="781" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A781" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B781" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C781" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E781" t="s">
+        <v>171</v>
+      </c>
+      <c r="F781" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="782" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A782" t="s">
+        <v>595</v>
+      </c>
+      <c r="B782" t="s">
+        <v>596</v>
+      </c>
+      <c r="C782" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E782" t="s">
+        <v>171</v>
+      </c>
+      <c r="F782" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="783" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A783" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B783" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C783" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E783" t="s">
+        <v>171</v>
+      </c>
+      <c r="F783" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="784" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A784" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B784" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C784" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E784" t="s">
+        <v>171</v>
+      </c>
+      <c r="F784" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A724:A747">
-    <sortCondition ref="A724"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A771:A784">
+    <sortCondition ref="A771"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1" xr:uid="{2726AE12-75BD-43F3-877F-718C53B6A31E}"/>
@@ -19192,8 +20088,10 @@
     <hyperlink ref="B335" r:id="rId21" xr:uid="{A0C56171-B818-446C-B795-9CE1959A6BB4}"/>
     <hyperlink ref="B424" r:id="rId22" xr:uid="{D1BF80C7-A4E5-4726-B423-A8554E853A45}"/>
     <hyperlink ref="B711" r:id="rId23" xr:uid="{1DB4C5A1-65C6-497B-AC49-2C13AA1FC146}"/>
+    <hyperlink ref="B770" r:id="rId24" xr:uid="{A4C7122C-1E7B-462A-AD13-52551FC281A2}"/>
+    <hyperlink ref="B771" r:id="rId25" xr:uid="{B93F069A-7583-419B-B11E-F3B4B1BF7471}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wii e Xbox perdidos
</commit_message>
<xml_diff>
--- a/jogos.xlsx
+++ b/jogos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\mycollections-cli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3516F148-6895-4411-9EC9-7C7280DE5181}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09ECBBD3-2570-47C4-AECC-9EFAA775A786}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{0C35237A-6EB4-4B02-9651-931FED775CEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3911" uniqueCount="1521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4001" uniqueCount="1556">
   <si>
     <t>Dragon Age Origins</t>
   </si>
@@ -4588,6 +4588,111 @@
   </si>
   <si>
     <t>PRO EVOLUTION SOCCER 2016</t>
+  </si>
+  <si>
+    <t>Gears of War</t>
+  </si>
+  <si>
+    <t>Gears of War 2</t>
+  </si>
+  <si>
+    <t>Gears of War 3</t>
+  </si>
+  <si>
+    <t>Gears of War Judgement</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTuCOqWFQ10b3zOq9O8OyfQtS2LD_sd0rP3Ip4iRX4oep69Xwc0</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSVNIHJw8-XsYsAGaNK6tNtE0UAD-Qrz1Cp7SfKbqnK3ichiXTC</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTWb0ricljrhot41Tm1hBKid157iphAndcjfeSnPBGDwY7Ks-g7Fw</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRlvwhwLXvywBXo7kOkxYBOrTggBs-xs2FtYtzWGHhoVm7Jz3X55Q</t>
+  </si>
+  <si>
+    <t>Assassins Creed Unity</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTcp6x7rM0N3sre7cHNSiv66VRKWGz_npaG7MbFMq06iloqK3-z</t>
+  </si>
+  <si>
+    <t>Mario Kart</t>
+  </si>
+  <si>
+    <t>Donkey Kong Country Returns</t>
+  </si>
+  <si>
+    <t>The Legend of Zelda Twilight Princess</t>
+  </si>
+  <si>
+    <t>The Last Story</t>
+  </si>
+  <si>
+    <t>Wii Sports Resort</t>
+  </si>
+  <si>
+    <t>New Super Mario Bros Wii</t>
+  </si>
+  <si>
+    <t>Super Mario Galaxy</t>
+  </si>
+  <si>
+    <t>Pikmin 2</t>
+  </si>
+  <si>
+    <t>Super Paper Mario</t>
+  </si>
+  <si>
+    <t>The Legend of Zelda Skyward Sword</t>
+  </si>
+  <si>
+    <t>Wii Sports</t>
+  </si>
+  <si>
+    <t>Super Mario Galaxy 2</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTJhjYxcs0DSUxaCjTRTRQXeJtPzjnUTbQe7rqckOBYUymXuur2</t>
+  </si>
+  <si>
+    <t>Wii</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSbwqWLNZS7t5txSQ_J4QnOTTUQp19tdyf6lIsJwP6XRbmMUihV</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcR7kJCv5tK9CHK6WCEcpv7cFyRHeRJehX4it4-oFyVejYawpR-gjw</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSMnHlTIyYkstE9M9XFTVz9HmTdwRgP0nHjj_9C-OGNkSuo16kTlg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQZAb6EFYyMel2Vs6HtrFksXLTAROFPeQ9tpS5iNYubKS1LImsb</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSIHeicEMJFtogkX0mzINLEi2P_KJ3B4JtXxh44-UcXe-gbCgJW</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTFHG5N3acPGb1NW2R3LYG-nY5tvZnDLEs2hYsrxS-atIsS0UmLdQ</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTTTwDR4q2bqlSOuP3q3M8eRVJXFH6FKzfsQH6yX1d7JWttSbDD</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQLpB6nukw_R5S_f19hKMjs1Jiadp74wSofWxvDszN9V60T2S-C</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRBOH61IB-_qkPZI7sVkVi_3yKdpG-KL-F3qUvVOjIlI21Zl8WqNQ</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcS7v5-aEv5YciskPBhO__KnXNelmyFdr-4AyqMYy63A-DwazsKAWA</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTdpmEhrBIB59nSV1jD6wqI1jUzwwF12JSMiEWt2g_FXCUOoXxs</t>
   </si>
 </sst>
 </file>
@@ -4959,10 +5064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E073D1A-5126-4785-A652-5C66939BBDE3}">
-  <dimension ref="A1:F784"/>
+  <dimension ref="A1:F802"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A761" workbookViewId="0">
-      <selection activeCell="A780" sqref="A780"/>
+    <sheetView tabSelected="1" topLeftCell="A766" workbookViewId="0">
+      <selection activeCell="B803" sqref="B803"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20051,9 +20156,315 @@
         <v>229</v>
       </c>
     </row>
+    <row r="785" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A785" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B785" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C785" t="s">
+        <v>162</v>
+      </c>
+      <c r="E785" t="s">
+        <v>170</v>
+      </c>
+      <c r="F785" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="786" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A786" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B786" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C786" t="s">
+        <v>162</v>
+      </c>
+      <c r="E786" t="s">
+        <v>170</v>
+      </c>
+      <c r="F786" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="787" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A787" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B787" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C787" t="s">
+        <v>162</v>
+      </c>
+      <c r="E787" t="s">
+        <v>170</v>
+      </c>
+      <c r="F787" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="788" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A788" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B788" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C788" t="s">
+        <v>162</v>
+      </c>
+      <c r="E788" t="s">
+        <v>170</v>
+      </c>
+      <c r="F788" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="789" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A789" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B789" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C789" t="s">
+        <v>162</v>
+      </c>
+      <c r="E789" t="s">
+        <v>170</v>
+      </c>
+      <c r="F789" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="790" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A790" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B790" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C790" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E790" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F790" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="791" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A791" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B791" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C791" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E791" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F791" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="792" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A792" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B792" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C792" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E792" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F792" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="793" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A793" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B793" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C793" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E793" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F793" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="794" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A794" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B794" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C794" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E794" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F794" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="795" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A795" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B795" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C795" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E795" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F795" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="796" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A796" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B796" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C796" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E796" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F796" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="797" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A797" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B797" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C797" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E797" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F797" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="798" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A798" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B798" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C798" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E798" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F798" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="799" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A799" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B799" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C799" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E799" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F799" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="800" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A800" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B800" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C800" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E800" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F800" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="801" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A801" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B801" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C801" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E801" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F801" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="802" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A802" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B802" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C802" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E802" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F802" t="s">
+        <v>229</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A771:A784">
-    <sortCondition ref="A771"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A790:A802">
+    <sortCondition ref="A790"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1" xr:uid="{2726AE12-75BD-43F3-877F-718C53B6A31E}"/>

</xml_diff>